<commit_message>
adding data structures pom and step definition files
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data/TestData.xlsx
+++ b/src/test/resources/test_data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sathizk7/eclipse-workspace/DS-ALGO/src/test/resources/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80364468-1EE4-944F-8584-34E854E3AC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F1562B-943C-7043-A37E-0E49C855334B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{492EBD1C-3B98-1F48-BBC4-B1ADEDF15E21}"/>
   </bookViews>
@@ -37,13 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
-  <si>
-    <t>valid</t>
-  </si>
-  <si>
-    <t>invalid</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>print "numpy"</t>
   </si>
@@ -51,9 +45,6 @@
     <t>print "ninja"</t>
   </si>
   <si>
-    <t>print "numpy":</t>
-  </si>
-  <si>
     <t>print "ninja":</t>
   </si>
   <si>
@@ -94,13 +85,28 @@
   </si>
   <si>
     <t>Please check your password</t>
+  </si>
+  <si>
+    <t>numpy</t>
+  </si>
+  <si>
+    <t>ninja</t>
+  </si>
+  <si>
+    <t>Valid code</t>
+  </si>
+  <si>
+    <t>Result for valid code</t>
+  </si>
+  <si>
+    <t>Invalid code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -116,6 +122,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -125,7 +138,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -133,14 +146,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -479,7 +509,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,73 +521,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D5" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -570,40 +600,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E76B54-6677-5142-881A-FB69C6344294}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing test data excel to avoid duplicate defect
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data/TestData.xlsx
+++ b/src/test/resources/test_data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sathizk7/eclipse-workspace/DS-ALGO/src/test/resources/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F1562B-943C-7043-A37E-0E49C855334B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F754296B-BBF7-834B-8A1C-19DC22F9C5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{492EBD1C-3B98-1F48-BBC4-B1ADEDF15E21}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>print "numpy"</t>
   </si>
@@ -166,11 +166,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -509,7 +510,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -577,18 +578,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>